<commit_message>
delete lead function created and respective changes done in other functions
</commit_message>
<xml_diff>
--- a/coreapi/coreapi/v0/ui/leads/lead_form_2.xlsx
+++ b/coreapi/coreapi/v0/ui/leads/lead_form_2.xlsx
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t xml:space="preserve">Supplier ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
   <si>
     <t xml:space="preserve">BENBLDBHRSAPR</t>
   </si>
@@ -127,10 +136,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -146,18 +155,29 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="n">
-        <v>31</v>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
delete lead form and delete lead entry functions added
</commit_message>
<xml_diff>
--- a/coreapi/coreapi/v0/ui/leads/lead_form_2.xlsx
+++ b/coreapi/coreapi/v0/ui/leads/lead_form_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Supplier ID</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Age</t>
+    <t xml:space="preserve">City</t>
   </si>
   <si>
     <t xml:space="preserve">BENBLDBHRSAPR</t>
@@ -37,10 +37,16 @@
     <t xml:space="preserve">Kushagra</t>
   </si>
   <si>
+    <t xml:space="preserve">Bharatpur</t>
+  </si>
+  <si>
     <t xml:space="preserve">GZBININRSGCC</t>
   </si>
   <si>
     <t xml:space="preserve">K2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangalore</t>
   </si>
 </sst>
 </file>
@@ -55,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,7 +146,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -166,19 +173,19 @@
       <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>31</v>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>